<commit_message>
Transfer some input parameters to json
To minimize any confusion, now the model read from Parameters.jason:
mean_acquisition_rate: the Average Daily Total
simulation_time: number of simulation DAYS
number_of_replications: number of simulation replications
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -472,34 +472,34 @@
         <v>6</v>
       </c>
       <c r="B2" s="2">
-        <v>14478</v>
+        <v>14405.5</v>
       </c>
       <c r="C2" s="2">
-        <v>14478</v>
+        <v>14405.5</v>
       </c>
       <c r="D2" s="2">
-        <v>0.570381751566009</v>
+        <v>0.573147927110687</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
       </c>
       <c r="F2" s="2">
-        <v>14478</v>
+        <v>14405.5</v>
       </c>
       <c r="G2" s="2">
-        <v>14478</v>
+        <v>14405.5</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="2">
-        <v>940</v>
+        <v>997</v>
       </c>
       <c r="K2" s="2">
-        <v>338</v>
+        <v>314.5</v>
       </c>
       <c r="L2" s="2">
-        <v>186</v>
+        <v>170.5</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>6</v>
@@ -511,7 +511,7 @@
         <v>0</v>
       </c>
       <c r="Q2" s="2">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -519,22 +519,22 @@
         <v>7</v>
       </c>
       <c r="B3" s="2">
-        <v>4369</v>
+        <v>4266</v>
       </c>
       <c r="C3" s="2">
-        <v>4369</v>
+        <v>4266</v>
       </c>
       <c r="D3" s="2">
-        <v>0.17212307449868</v>
+        <v>0.169730245882072</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
       </c>
       <c r="F3" s="2">
-        <v>4369</v>
+        <v>4266</v>
       </c>
       <c r="G3" s="2">
-        <v>4369</v>
+        <v>4266</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>7</v>
@@ -543,10 +543,10 @@
         <v>0</v>
       </c>
       <c r="K3" s="2">
-        <v>943</v>
+        <v>921</v>
       </c>
       <c r="L3" s="2">
-        <v>504</v>
+        <v>458</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>7</v>
@@ -555,10 +555,10 @@
         <v>0</v>
       </c>
       <c r="P3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -566,22 +566,22 @@
         <v>8</v>
       </c>
       <c r="B4" s="2">
-        <v>1277</v>
+        <v>1259</v>
       </c>
       <c r="C4" s="2">
-        <v>1277</v>
+        <v>1259</v>
       </c>
       <c r="D4" s="2">
-        <v>0.0503092621045582</v>
+        <v>0.0500915095090316</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
       </c>
       <c r="F4" s="2">
-        <v>1277</v>
+        <v>1259</v>
       </c>
       <c r="G4" s="2">
-        <v>1277</v>
+        <v>1259</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>8</v>
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="2">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L4" s="2">
         <v>0</v>
@@ -613,22 +613,22 @@
         <v>9</v>
       </c>
       <c r="B5" s="2">
-        <v>3000</v>
+        <v>2962</v>
       </c>
       <c r="C5" s="2">
-        <v>3000</v>
+        <v>2962</v>
       </c>
       <c r="D5" s="2">
-        <v>0.118189339321593</v>
+        <v>0.117848332935466</v>
       </c>
       <c r="E5" s="2">
         <v>1</v>
       </c>
       <c r="F5" s="2">
-        <v>3000</v>
+        <v>2962</v>
       </c>
       <c r="G5" s="2">
-        <v>3000</v>
+        <v>2962</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>9</v>
@@ -637,10 +637,10 @@
         <v>0</v>
       </c>
       <c r="K5" s="2">
-        <v>631</v>
+        <v>616</v>
       </c>
       <c r="L5" s="2">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>9</v>
@@ -649,10 +649,10 @@
         <v>0</v>
       </c>
       <c r="P5" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="2">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -660,34 +660,34 @@
         <v>10</v>
       </c>
       <c r="B6" s="2">
-        <v>2259</v>
+        <v>2241.5</v>
       </c>
       <c r="C6" s="2">
-        <v>2259</v>
+        <v>2241.5</v>
       </c>
       <c r="D6" s="2">
-        <v>0.0889965725091597</v>
+        <v>0.0891819845627437</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
       </c>
       <c r="F6" s="2">
-        <v>2259</v>
+        <v>2241.5</v>
       </c>
       <c r="G6" s="2">
-        <v>2259</v>
+        <v>2241.5</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J6" s="2">
-        <v>184</v>
+        <v>162.5</v>
       </c>
       <c r="K6" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L6" s="2">
-        <v>30</v>
+        <v>28.5</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>10</v>

</xml_diff>